<commit_message>
HOMEACC-31: #time 0h 5m Correct minor data
</commit_message>
<xml_diff>
--- a/trial/MeoDemo_Final/ImportFiles/Manual_Balance_202108.xlsx
+++ b/trial/MeoDemo_Final/ImportFiles/Manual_Balance_202108.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\miph272640\PycharmProjects\HomeAccounting\trial\MeoDemo_Final\ImportFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFC5B839-535B-44F3-A754-FF94D4C89445}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21E405C6-A70B-4B5E-A867-ECC04C4531A3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{211A79C5-B985-E94E-B0C1-2BF2BF8B9373}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{211A79C5-B985-E94E-B0C1-2BF2BF8B9373}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -3202,8 +3202,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C746422B-7B49-664B-A814-9E0769654701}">
   <dimension ref="A1:O1222"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1213" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A1220" sqref="A1220:E1222"/>
+    <sheetView tabSelected="1" topLeftCell="A1129" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A1151" sqref="A1151"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="19.5" x14ac:dyDescent="0.4"/>
@@ -33297,7 +33297,7 @@
     </row>
     <row r="1150" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A1150" s="11">
-        <v>44407</v>
+        <v>44438</v>
       </c>
       <c r="B1150" s="5" t="s">
         <v>117</v>
@@ -35649,7 +35649,7 @@
     <row r="3" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A3" s="11">
         <f ca="1">DATE(YEAR(TODAY()),MONTH(TODAY()),27)</f>
-        <v>44435</v>
+        <v>44466</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>160</v>
@@ -35671,7 +35671,7 @@
     <row r="4" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A4" s="11">
         <f ca="1">DATE(YEAR(TODAY()),MONTH(TODAY()),27)</f>
-        <v>44435</v>
+        <v>44466</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>313</v>
@@ -35692,7 +35692,7 @@
     <row r="5" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A5" s="11">
         <f ca="1">DATE(YEAR(TODAY()),MONTH(TODAY()),27)</f>
-        <v>44435</v>
+        <v>44466</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>435</v>
@@ -35713,7 +35713,7 @@
     <row r="6" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A6" s="11">
         <f ca="1">DATE(YEAR(TODAY()),MONTH(TODAY()),27)</f>
-        <v>44435</v>
+        <v>44466</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>315</v>
@@ -35734,7 +35734,7 @@
     <row r="7" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A7" s="11">
         <f t="shared" ref="A7:A10" ca="1" si="0">DATE(YEAR(TODAY()),MONTH(TODAY()),27)</f>
-        <v>44435</v>
+        <v>44466</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>164</v>
@@ -35755,7 +35755,7 @@
     <row r="8" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A8" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>44435</v>
+        <v>44466</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>316</v>
@@ -35776,7 +35776,7 @@
     <row r="9" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A9" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>44435</v>
+        <v>44466</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>314</v>
@@ -35797,7 +35797,7 @@
     <row r="10" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A10" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>44435</v>
+        <v>44466</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>317</v>
@@ -35818,7 +35818,7 @@
     <row r="11" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A11" s="11">
         <f t="shared" ref="A11:A14" ca="1" si="1">DATE(YEAR(TODAY()),MONTH(TODAY()),27)</f>
-        <v>44435</v>
+        <v>44466</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>179</v>
@@ -35839,7 +35839,7 @@
     <row r="12" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A12" s="11">
         <f t="shared" ca="1" si="1"/>
-        <v>44435</v>
+        <v>44466</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>428</v>
@@ -35860,7 +35860,7 @@
     <row r="13" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A13" s="11">
         <f t="shared" ca="1" si="1"/>
-        <v>44435</v>
+        <v>44466</v>
       </c>
       <c r="B13" s="5" t="s">
         <v>431</v>
@@ -35881,7 +35881,7 @@
     <row r="14" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A14" s="11">
         <f t="shared" ca="1" si="1"/>
-        <v>44435</v>
+        <v>44466</v>
       </c>
       <c r="B14" s="5" t="s">
         <v>430</v>
@@ -35902,7 +35902,7 @@
     <row r="15" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A15" s="11">
         <f ca="1">DATE(YEAR(TODAY()),MONTH(TODAY()),15)</f>
-        <v>44423</v>
+        <v>44454</v>
       </c>
       <c r="B15" s="7" t="s">
         <v>456</v>
@@ -35938,7 +35938,7 @@
     <row r="16" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A16" s="11">
         <f ca="1">DATE(YEAR(TODAY()),MONTH(TODAY()),25)</f>
-        <v>44433</v>
+        <v>44464</v>
       </c>
       <c r="B16" s="7" t="s">
         <v>304</v>
@@ -35959,11 +35959,11 @@
     <row r="17" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A17" s="11">
         <f ca="1">DATE(YEAR(TODAY()),MONTH(TODAY()),25)</f>
-        <v>44433</v>
+        <v>44464</v>
       </c>
       <c r="B17" s="5" t="str">
         <f ca="1">CONCATENATE("House rental 2021.",TEXT(MONTH(A17),"00"))</f>
-        <v>House rental 2021.08</v>
+        <v>House rental 2021.09</v>
       </c>
       <c r="C17" s="12">
         <v>121000</v>
@@ -35999,7 +35999,7 @@
     <row r="18" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A18" s="11">
         <f ca="1">DATE(YEAR(TODAY()),MONTH(TODAY()),26)</f>
-        <v>44434</v>
+        <v>44465</v>
       </c>
       <c r="B18" s="5" t="str">
         <f>CONCATENATE("Kindergarten Puppy 2021.",TEXT(MONTH(A24),"00"))</f>
@@ -36039,7 +36039,7 @@
     <row r="19" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A19" s="11">
         <f ca="1">DATE(YEAR(TODAY()),MONTH(TODAY()),26)</f>
-        <v>44434</v>
+        <v>44465</v>
       </c>
       <c r="B19" s="5" t="s">
         <v>447</v>
@@ -36060,7 +36060,7 @@
     <row r="20" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A20" s="11">
         <f ca="1">DATE(YEAR(TODAY()),MONTH(TODAY()),26)</f>
-        <v>44434</v>
+        <v>44465</v>
       </c>
       <c r="B20" s="5" t="s">
         <v>450</v>
@@ -36081,7 +36081,7 @@
     <row r="21" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A21" s="11">
         <f ca="1">DATE(YEAR(TODAY()),MONTH(TODAY()),26)</f>
-        <v>44434</v>
+        <v>44465</v>
       </c>
       <c r="B21" s="5" t="s">
         <v>451</v>

</xml_diff>